<commit_message>
atualizações e adição de sql
</commit_message>
<xml_diff>
--- a/tabelas-mkdocs.xlsx
+++ b/tabelas-mkdocs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" tabRatio="841" firstSheet="4" activeTab="12"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" tabRatio="841" firstSheet="4" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="procv" sheetId="1" r:id="rId1"/>
@@ -17,25 +17,27 @@
     <sheet name="soma.se_2" sheetId="5" r:id="rId8"/>
     <sheet name="cont.ses" sheetId="2" r:id="rId9"/>
     <sheet name="cont.se" sheetId="3" r:id="rId10"/>
-    <sheet name="tabela_dinamica" sheetId="12" r:id="rId11"/>
-    <sheet name="grafico_dinamico" sheetId="19" r:id="rId12"/>
-    <sheet name="base_de_dados" sheetId="22" r:id="rId13"/>
-    <sheet name="dashboard" sheetId="21" r:id="rId14"/>
+    <sheet name="gráfico" sheetId="23" r:id="rId11"/>
+    <sheet name="tabela_dinamica" sheetId="12" r:id="rId12"/>
+    <sheet name="grafico_dinamico" sheetId="19" r:id="rId13"/>
+    <sheet name="base_de_dados" sheetId="22" r:id="rId14"/>
+    <sheet name="dashboard" sheetId="21" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="quantidade">procv!$B$2:$B$11</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId15"/>
-    <pivotCache cacheId="1" r:id="rId16"/>
-    <pivotCache cacheId="6" r:id="rId17"/>
+    <pivotCache cacheId="0" r:id="rId16"/>
+    <pivotCache cacheId="1" r:id="rId17"/>
+    <pivotCache cacheId="2" r:id="rId18"/>
   </pivotCaches>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="165">
   <si>
     <t>Descrição</t>
   </si>
@@ -524,6 +526,12 @@
   </si>
   <si>
     <t>Fevereiro</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -771,6 +779,198 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>gráfico!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>gráfico!$B$1:$N$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>gráfico!$B$2:$N$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>190</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="196469888"/>
+        <c:axId val="196469312"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="196469888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="196469312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="196469312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="196469888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="118"/>
     </mc:Choice>
     <mc:Fallback>
@@ -798,7 +998,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1063,11 +1262,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="127639040"/>
-        <c:axId val="182786240"/>
+        <c:axId val="191808000"/>
+        <c:axId val="162586624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="127639040"/>
+        <c:axId val="191808000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1076,7 +1275,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182786240"/>
+        <c:crossAx val="162586624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1084,7 +1283,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182786240"/>
+        <c:axId val="162586624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1095,7 +1294,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127639040"/>
+        <c:crossAx val="191808000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1108,7 +1307,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1131,7 +1329,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
@@ -1356,11 +1554,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="191846400"/>
-        <c:axId val="182787392"/>
+        <c:axId val="135860736"/>
+        <c:axId val="162588352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="191846400"/>
+        <c:axId val="135860736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1369,7 +1567,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182787392"/>
+        <c:crossAx val="162588352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1377,7 +1575,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182787392"/>
+        <c:axId val="162588352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1388,14 +1586,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191846400"/>
+        <c:crossAx val="135860736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1422,6 +1619,41 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1456,7 +1688,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2053,7 +2285,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="E1:I7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisCol" showAll="0">
@@ -2863,6 +3095,117 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="6.7109375" style="2" customWidth="1"/>
+    <col min="5" max="14" width="6.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="14">
+        <v>5</v>
+      </c>
+      <c r="C1" s="14">
+        <v>120</v>
+      </c>
+      <c r="D1" s="14">
+        <v>17</v>
+      </c>
+      <c r="E1" s="14">
+        <v>40</v>
+      </c>
+      <c r="F1" s="14">
+        <v>33</v>
+      </c>
+      <c r="G1" s="14">
+        <v>135</v>
+      </c>
+      <c r="H1" s="14">
+        <v>90</v>
+      </c>
+      <c r="I1" s="14">
+        <v>180</v>
+      </c>
+      <c r="J1" s="14">
+        <v>70</v>
+      </c>
+      <c r="K1" s="14">
+        <v>159</v>
+      </c>
+      <c r="L1" s="14">
+        <v>110</v>
+      </c>
+      <c r="M1" s="14">
+        <v>60</v>
+      </c>
+      <c r="N1" s="14">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="14">
+        <v>10</v>
+      </c>
+      <c r="C2" s="14">
+        <v>135</v>
+      </c>
+      <c r="D2" s="14">
+        <v>20</v>
+      </c>
+      <c r="E2" s="14">
+        <v>60</v>
+      </c>
+      <c r="F2" s="14">
+        <v>40</v>
+      </c>
+      <c r="G2" s="14">
+        <v>160</v>
+      </c>
+      <c r="H2" s="14">
+        <v>105</v>
+      </c>
+      <c r="I2" s="14">
+        <v>180</v>
+      </c>
+      <c r="J2" s="14">
+        <v>100</v>
+      </c>
+      <c r="K2" s="14">
+        <v>165</v>
+      </c>
+      <c r="L2" s="14">
+        <v>115</v>
+      </c>
+      <c r="M2" s="14">
+        <v>70</v>
+      </c>
+      <c r="N2" s="14">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3107,7 +3450,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -3382,11 +3725,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -3646,7 +3989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>